<commit_message>
Check if scripts are working
</commit_message>
<xml_diff>
--- a/Experimental_scripts/Lists/repswitch_V2L4.xlsx
+++ b/Experimental_scripts/Lists/repswitch_V2L4.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27231"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\experiment1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\experiment1\Experimental_scripts\Lists\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42F7D0C1-C919-49A2-9077-86F777D51CD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1D86923-A5CF-404F-B5A6-C62CB70CE6B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10080" yWindow="600" windowWidth="12960" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="11" r:id="rId1"/>
@@ -341,124 +341,124 @@
     <t>aguja</t>
   </si>
   <si>
-    <t>REPSWITCH1/PICTURE_8.png</t>
-  </si>
-  <si>
-    <t>REPSWITCH1/PICTURE_498.png</t>
-  </si>
-  <si>
-    <t>REPSWITCH1/PICTURE_19.png</t>
-  </si>
-  <si>
-    <t>REPSWITCH1/PICTURE_319.png</t>
-  </si>
-  <si>
-    <t>REPSWITCH1/PICTURE_169.png</t>
-  </si>
-  <si>
-    <t>REPSWITCH1/PICTURE_728.png</t>
-  </si>
-  <si>
-    <t>REPSWITCH1/PICTURE_142.png</t>
-  </si>
-  <si>
-    <t>REPSWITCH1/PICTURE_338.png</t>
-  </si>
-  <si>
-    <t>REPSWITCH1/PICTURE_135.png</t>
-  </si>
-  <si>
-    <t>REPSWITCH1/PICTURE_48.png</t>
-  </si>
-  <si>
-    <t>REPSWITCH1/PICTURE_687.png</t>
-  </si>
-  <si>
-    <t>REPSWITCH1/PICTURE_128.png</t>
-  </si>
-  <si>
-    <t>REPSWITCH1/PICTURE_719.png</t>
-  </si>
-  <si>
-    <t>REPSWITCH1/PICTURE_178.png</t>
-  </si>
-  <si>
-    <t>REPSWITCH1/PICTURE_16.png</t>
-  </si>
-  <si>
-    <t>REPSWITCH1/PICTURE_199.png</t>
-  </si>
-  <si>
-    <t>REPSWITCH1/PICTURE_517.png</t>
-  </si>
-  <si>
-    <t>REPSWITCH1/PICTURE_673.png</t>
-  </si>
-  <si>
-    <t>REPSWITCH1/PICTURE_552.png</t>
-  </si>
-  <si>
-    <t>REPSWITCH1/PICTURE_152.png</t>
-  </si>
-  <si>
-    <t>REPSWITCH1/PICTURE_446.png</t>
-  </si>
-  <si>
-    <t>REPSWITCH1/PICTURE_264.png</t>
-  </si>
-  <si>
-    <t>REPSWITCH1/PICTURE_30.png</t>
-  </si>
-  <si>
-    <t>REPSWITCH1/PICTURE_646.png</t>
-  </si>
-  <si>
-    <t>REPSWITCH1/PICTURE_175.png</t>
-  </si>
-  <si>
-    <t>REPSWITCH1/PICTURE_663.png</t>
-  </si>
-  <si>
-    <t>REPSWITCH1/PICTURE_35.png</t>
-  </si>
-  <si>
-    <t>REPSWITCH1/PICTURE_576.png</t>
-  </si>
-  <si>
-    <t>REPSWITCH1/PICTURE_271.png</t>
-  </si>
-  <si>
-    <t>REPSWITCH1/PICTURE_242.png</t>
-  </si>
-  <si>
-    <t>REPSWITCH1/PICTURE_610.png</t>
-  </si>
-  <si>
-    <t>REPSWITCH1/PICTURE_320.png</t>
-  </si>
-  <si>
-    <t>REPSWITCH1/PICTURE_464.png</t>
-  </si>
-  <si>
-    <t>REPSWITCH1/PICTURE_235.png</t>
-  </si>
-  <si>
-    <t>REPSWITCH1/PICTURE_340.png</t>
-  </si>
-  <si>
-    <t>REPSWITCH1/PICTURE_391.png</t>
-  </si>
-  <si>
-    <t>REPSWITCH1/PICTURE_590.png</t>
-  </si>
-  <si>
-    <t>REPSWITCH1/PICTURE_381.png</t>
-  </si>
-  <si>
     <t>fresa</t>
   </si>
   <si>
     <t>trial_no</t>
+  </si>
+  <si>
+    <t>Pictures/PICTURE_8.png</t>
+  </si>
+  <si>
+    <t>Pictures/PICTURE_498.png</t>
+  </si>
+  <si>
+    <t>Pictures/PICTURE_19.png</t>
+  </si>
+  <si>
+    <t>Pictures/PICTURE_319.png</t>
+  </si>
+  <si>
+    <t>Pictures/PICTURE_169.png</t>
+  </si>
+  <si>
+    <t>Pictures/PICTURE_728.png</t>
+  </si>
+  <si>
+    <t>Pictures/PICTURE_142.png</t>
+  </si>
+  <si>
+    <t>Pictures/PICTURE_338.png</t>
+  </si>
+  <si>
+    <t>Pictures/PICTURE_135.png</t>
+  </si>
+  <si>
+    <t>Pictures/PICTURE_381.png</t>
+  </si>
+  <si>
+    <t>Pictures/PICTURE_48.png</t>
+  </si>
+  <si>
+    <t>Pictures/PICTURE_687.png</t>
+  </si>
+  <si>
+    <t>Pictures/PICTURE_128.png</t>
+  </si>
+  <si>
+    <t>Pictures/PICTURE_719.png</t>
+  </si>
+  <si>
+    <t>Pictures/PICTURE_178.png</t>
+  </si>
+  <si>
+    <t>Pictures/PICTURE_16.png</t>
+  </si>
+  <si>
+    <t>Pictures/PICTURE_199.png</t>
+  </si>
+  <si>
+    <t>Pictures/PICTURE_517.png</t>
+  </si>
+  <si>
+    <t>Pictures/PICTURE_673.png</t>
+  </si>
+  <si>
+    <t>Pictures/PICTURE_552.png</t>
+  </si>
+  <si>
+    <t>Pictures/PICTURE_152.png</t>
+  </si>
+  <si>
+    <t>Pictures/PICTURE_446.png</t>
+  </si>
+  <si>
+    <t>Pictures/PICTURE_264.png</t>
+  </si>
+  <si>
+    <t>Pictures/PICTURE_30.png</t>
+  </si>
+  <si>
+    <t>Pictures/PICTURE_646.png</t>
+  </si>
+  <si>
+    <t>Pictures/PICTURE_175.png</t>
+  </si>
+  <si>
+    <t>Pictures/PICTURE_663.png</t>
+  </si>
+  <si>
+    <t>Pictures/PICTURE_35.png</t>
+  </si>
+  <si>
+    <t>Pictures/PICTURE_576.png</t>
+  </si>
+  <si>
+    <t>Pictures/PICTURE_271.png</t>
+  </si>
+  <si>
+    <t>Pictures/PICTURE_242.png</t>
+  </si>
+  <si>
+    <t>Pictures/PICTURE_610.png</t>
+  </si>
+  <si>
+    <t>Pictures/PICTURE_320.png</t>
+  </si>
+  <si>
+    <t>Pictures/PICTURE_464.png</t>
+  </si>
+  <si>
+    <t>Pictures/PICTURE_235.png</t>
+  </si>
+  <si>
+    <t>Pictures/PICTURE_340.png</t>
+  </si>
+  <si>
+    <t>Pictures/PICTURE_391.png</t>
+  </si>
+  <si>
+    <t>Pictures/PICTURE_590.png</t>
   </si>
 </sst>
 </file>
@@ -1464,7 +1464,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5316FD7-5512-4A07-AE9D-CE20BFD960BD}">
   <dimension ref="A1:Q409"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A388" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A387" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E413" sqref="E413"/>
     </sheetView>
   </sheetViews>
@@ -1517,7 +1517,7 @@
         <v>60</v>
       </c>
       <c r="O1" s="5" t="s">
-        <v>141</v>
+        <v>103</v>
       </c>
       <c r="P1" s="5" t="s">
         <v>58</v>
@@ -1528,7 +1528,7 @@
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="22" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>71</v>
@@ -1579,7 +1579,7 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="22" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>72</v>
@@ -1630,7 +1630,7 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="22" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>73</v>
@@ -1683,7 +1683,7 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="22" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>73</v>
@@ -1734,7 +1734,7 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="22" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>74</v>
@@ -1787,7 +1787,7 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="22" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>75</v>
@@ -1840,7 +1840,7 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="22" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>75</v>
@@ -1891,7 +1891,7 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="22" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>76</v>
@@ -1942,7 +1942,7 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" s="22" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>77</v>
@@ -1995,7 +1995,7 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="22" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>77</v>
@@ -2046,7 +2046,7 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="22" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>78</v>
@@ -2099,7 +2099,7 @@
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="22" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>79</v>
@@ -2152,7 +2152,7 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" s="22" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>79</v>
@@ -2203,10 +2203,10 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" s="22" t="s">
-        <v>139</v>
+        <v>113</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>140</v>
+        <v>102</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>1</v>
@@ -2256,10 +2256,10 @@
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" s="22" t="s">
-        <v>139</v>
+        <v>113</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>140</v>
+        <v>102</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>2</v>
@@ -2307,7 +2307,7 @@
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="22" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>80</v>
@@ -2358,7 +2358,7 @@
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" s="22" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>81</v>
@@ -2409,7 +2409,7 @@
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" s="22" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>82</v>
@@ -2460,7 +2460,7 @@
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" s="22" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>82</v>
@@ -2511,7 +2511,7 @@
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21" s="22" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>83</v>
@@ -2564,7 +2564,7 @@
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22" s="22" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>84</v>
@@ -2617,7 +2617,7 @@
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23" s="22" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>84</v>
@@ -2668,7 +2668,7 @@
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24" s="22" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>85</v>
@@ -2721,7 +2721,7 @@
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A25" s="22" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>85</v>
@@ -2772,7 +2772,7 @@
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26" s="22" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>73</v>
@@ -2823,7 +2823,7 @@
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27" s="22" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>86</v>
@@ -2876,7 +2876,7 @@
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A28" s="22" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>86</v>
@@ -2927,7 +2927,7 @@
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A29" s="22" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>84</v>
@@ -2980,7 +2980,7 @@
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A30" s="22" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>87</v>
@@ -3033,7 +3033,7 @@
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A31" s="22" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>87</v>
@@ -3084,7 +3084,7 @@
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A32" s="22" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>75</v>
@@ -3135,7 +3135,7 @@
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A33" s="29" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="B33" s="30" t="s">
         <v>56</v>
@@ -3186,7 +3186,7 @@
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A34" s="22" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>77</v>
@@ -3239,7 +3239,7 @@
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A35" s="22" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>88</v>
@@ -3292,7 +3292,7 @@
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A36" s="22" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>88</v>
@@ -3343,7 +3343,7 @@
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A37" s="22" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>79</v>
@@ -3394,7 +3394,7 @@
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A38" s="22" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>89</v>
@@ -3447,7 +3447,7 @@
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A39" s="22" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>89</v>
@@ -3498,10 +3498,10 @@
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A40" s="22" t="s">
-        <v>139</v>
+        <v>113</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>140</v>
+        <v>102</v>
       </c>
       <c r="C40" s="6" t="s">
         <v>2</v>
@@ -3549,7 +3549,7 @@
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A41" s="22" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>90</v>
@@ -3602,7 +3602,7 @@
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A42" s="22" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>90</v>
@@ -3653,7 +3653,7 @@
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A43" s="22" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>91</v>
@@ -3704,7 +3704,7 @@
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A44" s="22" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>91</v>
@@ -3755,7 +3755,7 @@
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A45" s="22" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>82</v>
@@ -3806,7 +3806,7 @@
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A46" s="22" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>92</v>
@@ -3859,7 +3859,7 @@
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A47" s="22" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>92</v>
@@ -3910,7 +3910,7 @@
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A48" s="29" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="B48" s="30" t="s">
         <v>55</v>
@@ -3961,7 +3961,7 @@
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A49" s="22" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>85</v>
@@ -4012,7 +4012,7 @@
     </row>
     <row r="50" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A50" s="22" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>93</v>
@@ -4065,7 +4065,7 @@
     </row>
     <row r="51" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A51" s="22" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>93</v>
@@ -4116,7 +4116,7 @@
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A52" s="31" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="B52" s="32" t="s">
         <v>57</v>
@@ -4167,7 +4167,7 @@
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A53" s="22" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>94</v>
@@ -4218,7 +4218,7 @@
     </row>
     <row r="54" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A54" s="22" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>94</v>
@@ -4269,7 +4269,7 @@
     </row>
     <row r="55" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A55" s="22" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>86</v>
@@ -4320,7 +4320,7 @@
     </row>
     <row r="56" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A56" s="22" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>95</v>
@@ -4373,7 +4373,7 @@
     </row>
     <row r="57" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A57" s="22" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>95</v>
@@ -4424,7 +4424,7 @@
     </row>
     <row r="58" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A58" s="22" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>87</v>
@@ -4477,7 +4477,7 @@
     </row>
     <row r="59" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A59" s="22" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>96</v>
@@ -4530,7 +4530,7 @@
     </row>
     <row r="60" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A60" s="22" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>96</v>
@@ -4581,7 +4581,7 @@
     </row>
     <row r="61" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A61" s="22" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>88</v>
@@ -4632,7 +4632,7 @@
     </row>
     <row r="62" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A62" s="22" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>97</v>
@@ -4685,7 +4685,7 @@
     </row>
     <row r="63" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A63" s="22" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>97</v>
@@ -4736,7 +4736,7 @@
     </row>
     <row r="64" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A64" s="22" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>89</v>
@@ -4787,7 +4787,7 @@
     </row>
     <row r="65" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A65" s="22" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>90</v>
@@ -4840,7 +4840,7 @@
     </row>
     <row r="66" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A66" s="22" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>98</v>
@@ -4893,7 +4893,7 @@
     </row>
     <row r="67" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A67" s="22" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>98</v>
@@ -4944,7 +4944,7 @@
     </row>
     <row r="68" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A68" s="22" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>99</v>
@@ -4997,7 +4997,7 @@
     </row>
     <row r="69" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A69" s="22" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>99</v>
@@ -5048,7 +5048,7 @@
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A70" s="22" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>92</v>
@@ -5099,7 +5099,7 @@
     </row>
     <row r="71" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A71" s="22" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>91</v>
@@ -5150,7 +5150,7 @@
     </row>
     <row r="72" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A72" s="22" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>100</v>
@@ -5201,7 +5201,7 @@
     </row>
     <row r="73" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A73" s="22" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>100</v>
@@ -5252,7 +5252,7 @@
     </row>
     <row r="74" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A74" s="22" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>93</v>
@@ -5303,7 +5303,7 @@
     </row>
     <row r="75" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A75" s="22" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>101</v>
@@ -5356,7 +5356,7 @@
     </row>
     <row r="76" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A76" s="22" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>101</v>
@@ -5407,7 +5407,7 @@
     </row>
     <row r="77" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A77" s="22" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>95</v>
@@ -5460,7 +5460,7 @@
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A78" s="29" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="B78" s="30" t="s">
         <v>52</v>
@@ -5511,7 +5511,7 @@
     </row>
     <row r="79" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A79" s="22" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>100</v>
@@ -5564,7 +5564,7 @@
     </row>
     <row r="80" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A80" s="22" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>78</v>
@@ -5615,7 +5615,7 @@
     </row>
     <row r="81" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A81" s="22" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>78</v>
@@ -5666,7 +5666,7 @@
     </row>
     <row r="82" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A82" s="22" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>71</v>
@@ -5719,7 +5719,7 @@
     </row>
     <row r="83" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A83" s="22" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>71</v>
@@ -5770,7 +5770,7 @@
     </row>
     <row r="84" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A84" s="22" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>96</v>
@@ -5821,7 +5821,7 @@
     </row>
     <row r="85" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A85" s="22" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>81</v>
@@ -5874,7 +5874,7 @@
     </row>
     <row r="86" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A86" s="22" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>81</v>
@@ -5925,7 +5925,7 @@
     </row>
     <row r="87" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A87" s="22" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>74</v>
@@ -5976,7 +5976,7 @@
     </row>
     <row r="88" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A88" s="22" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>74</v>
@@ -6027,7 +6027,7 @@
     </row>
     <row r="89" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A89" s="22" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>97</v>
@@ -6078,7 +6078,7 @@
     </row>
     <row r="90" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A90" s="22" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>72</v>
@@ -6131,7 +6131,7 @@
     </row>
     <row r="91" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A91" s="22" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>72</v>
@@ -6182,7 +6182,7 @@
     </row>
     <row r="92" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A92" s="29" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="B92" s="30" t="s">
         <v>53</v>
@@ -6233,7 +6233,7 @@
     </row>
     <row r="93" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A93" s="22" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>98</v>
@@ -6284,7 +6284,7 @@
     </row>
     <row r="94" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A94" s="22" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>80</v>
@@ -6337,7 +6337,7 @@
     </row>
     <row r="95" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A95" s="22" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B95" s="1" t="s">
         <v>80</v>
@@ -6388,7 +6388,7 @@
     </row>
     <row r="96" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A96" s="22" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>99</v>
@@ -6441,7 +6441,7 @@
     </row>
     <row r="97" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A97" s="22" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>94</v>
@@ -6492,7 +6492,7 @@
     </row>
     <row r="98" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A98" s="22" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>76</v>
@@ -6545,7 +6545,7 @@
     </row>
     <row r="99" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A99" s="22" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B99" s="1" t="s">
         <v>76</v>
@@ -6596,7 +6596,7 @@
     </row>
     <row r="100" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A100" s="29" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="B100" s="30" t="s">
         <v>54</v>
@@ -6647,7 +6647,7 @@
     </row>
     <row r="101" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A101" s="22" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="B101" s="1" t="s">
         <v>101</v>
@@ -6698,7 +6698,7 @@
     </row>
     <row r="102" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A102" s="22" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="B102" s="1" t="s">
         <v>83</v>
@@ -6751,7 +6751,7 @@
     </row>
     <row r="103" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A103" s="23" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="B103" s="21" t="s">
         <v>83</v>
@@ -6802,7 +6802,7 @@
     </row>
     <row r="104" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A104" s="29" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="B104" s="30" t="s">
         <v>55</v>
@@ -6853,7 +6853,7 @@
     </row>
     <row r="105" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A105" s="29" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="B105" s="30" t="s">
         <v>52</v>
@@ -6904,7 +6904,7 @@
     </row>
     <row r="106" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A106" s="22" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B106" s="1" t="s">
         <v>78</v>
@@ -6955,7 +6955,7 @@
     </row>
     <row r="107" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A107" s="22" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B107" s="1" t="s">
         <v>77</v>
@@ -7008,7 +7008,7 @@
     </row>
     <row r="108" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A108" s="22" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B108" s="1" t="s">
         <v>77</v>
@@ -7059,7 +7059,7 @@
     </row>
     <row r="109" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A109" s="22" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B109" s="1" t="s">
         <v>72</v>
@@ -7110,7 +7110,7 @@
     </row>
     <row r="110" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A110" s="22" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="B110" s="1" t="s">
         <v>85</v>
@@ -7163,7 +7163,7 @@
     </row>
     <row r="111" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A111" s="22" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="B111" s="1" t="s">
         <v>85</v>
@@ -7214,7 +7214,7 @@
     </row>
     <row r="112" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A112" s="22" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="B112" s="1" t="s">
         <v>83</v>
@@ -7265,7 +7265,7 @@
     </row>
     <row r="113" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A113" s="22" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B113" s="1" t="s">
         <v>75</v>
@@ -7316,7 +7316,7 @@
     </row>
     <row r="114" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A114" s="22" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B114" s="1" t="s">
         <v>75</v>
@@ -7367,7 +7367,7 @@
     </row>
     <row r="115" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A115" s="22" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="B115" s="1" t="s">
         <v>81</v>
@@ -7418,7 +7418,7 @@
     </row>
     <row r="116" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A116" s="22" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="B116" s="1" t="s">
         <v>84</v>
@@ -7471,7 +7471,7 @@
     </row>
     <row r="117" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A117" s="22" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="B117" s="1" t="s">
         <v>84</v>
@@ -7522,7 +7522,7 @@
     </row>
     <row r="118" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A118" s="22" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B118" s="1" t="s">
         <v>82</v>
@@ -7575,7 +7575,7 @@
     </row>
     <row r="119" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A119" s="22" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B119" s="1" t="s">
         <v>82</v>
@@ -7626,7 +7626,7 @@
     </row>
     <row r="120" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A120" s="22" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B120" s="1" t="s">
         <v>74</v>
@@ -7679,7 +7679,7 @@
     </row>
     <row r="121" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A121" s="22" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B121" s="1" t="s">
         <v>76</v>
@@ -7730,10 +7730,10 @@
     </row>
     <row r="122" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A122" s="22" t="s">
-        <v>139</v>
+        <v>113</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>140</v>
+        <v>102</v>
       </c>
       <c r="C122" s="6" t="s">
         <v>2</v>
@@ -7783,10 +7783,10 @@
     </row>
     <row r="123" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A123" s="22" t="s">
-        <v>139</v>
+        <v>113</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>140</v>
+        <v>102</v>
       </c>
       <c r="C123" s="6" t="s">
         <v>2</v>
@@ -7834,7 +7834,7 @@
     </row>
     <row r="124" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A124" s="22" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B124" s="1" t="s">
         <v>71</v>
@@ -7885,7 +7885,7 @@
     </row>
     <row r="125" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A125" s="22" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B125" s="1" t="s">
         <v>80</v>
@@ -7936,7 +7936,7 @@
     </row>
     <row r="126" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A126" s="22" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B126" s="1" t="s">
         <v>79</v>
@@ -7989,7 +7989,7 @@
     </row>
     <row r="127" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A127" s="22" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B127" s="1" t="s">
         <v>79</v>
@@ -8040,7 +8040,7 @@
     </row>
     <row r="128" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A128" s="22" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B128" s="1" t="s">
         <v>73</v>
@@ -8093,7 +8093,7 @@
     </row>
     <row r="129" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A129" s="22" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B129" s="1" t="s">
         <v>73</v>
@@ -8144,7 +8144,7 @@
     </row>
     <row r="130" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A130" s="22" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B130" s="1" t="s">
         <v>77</v>
@@ -8195,7 +8195,7 @@
     </row>
     <row r="131" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A131" s="22" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B131" s="1" t="s">
         <v>79</v>
@@ -8246,7 +8246,7 @@
     </row>
     <row r="132" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A132" s="22" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="B132" s="1" t="s">
         <v>90</v>
@@ -8297,7 +8297,7 @@
     </row>
     <row r="133" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A133" s="22" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="B133" s="1" t="s">
         <v>90</v>
@@ -8348,7 +8348,7 @@
     </row>
     <row r="134" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A134" s="22" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="B134" s="1" t="s">
         <v>85</v>
@@ -8399,7 +8399,7 @@
     </row>
     <row r="135" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A135" s="22" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="B135" s="1" t="s">
         <v>88</v>
@@ -8452,7 +8452,7 @@
     </row>
     <row r="136" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A136" s="22" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="B136" s="1" t="s">
         <v>88</v>
@@ -8503,7 +8503,7 @@
     </row>
     <row r="137" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A137" s="22" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="B137" s="1" t="s">
         <v>87</v>
@@ -8554,7 +8554,7 @@
     </row>
     <row r="138" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A138" s="22" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="B138" s="1" t="s">
         <v>87</v>
@@ -8605,7 +8605,7 @@
     </row>
     <row r="139" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A139" s="22" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B139" s="1" t="s">
         <v>75</v>
@@ -8658,7 +8658,7 @@
     </row>
     <row r="140" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A140" s="22" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="B140" s="1" t="s">
         <v>92</v>
@@ -8711,7 +8711,7 @@
     </row>
     <row r="141" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A141" s="22" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="B141" s="1" t="s">
         <v>92</v>
@@ -8762,7 +8762,7 @@
     </row>
     <row r="142" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A142" s="22" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B142" s="1" t="s">
         <v>82</v>
@@ -8815,7 +8815,7 @@
     </row>
     <row r="143" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A143" s="22" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="B143" s="1" t="s">
         <v>86</v>
@@ -8866,7 +8866,7 @@
     </row>
     <row r="144" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A144" s="22" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="B144" s="1" t="s">
         <v>86</v>
@@ -8917,7 +8917,7 @@
     </row>
     <row r="145" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A145" s="22" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="B145" s="1" t="s">
         <v>89</v>
@@ -8970,7 +8970,7 @@
     </row>
     <row r="146" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A146" s="22" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="B146" s="1" t="s">
         <v>89</v>
@@ -9021,10 +9021,10 @@
     </row>
     <row r="147" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A147" s="22" t="s">
-        <v>139</v>
+        <v>113</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>140</v>
+        <v>102</v>
       </c>
       <c r="C147" s="6" t="s">
         <v>2</v>
@@ -9072,7 +9072,7 @@
     </row>
     <row r="148" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A148" s="22" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="B148" s="1" t="s">
         <v>93</v>
@@ -9125,7 +9125,7 @@
     </row>
     <row r="149" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A149" s="22" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="B149" s="1" t="s">
         <v>93</v>
@@ -9176,7 +9176,7 @@
     </row>
     <row r="150" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A150" s="22" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="B150" s="1" t="s">
         <v>84</v>
@@ -9227,7 +9227,7 @@
     </row>
     <row r="151" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A151" s="22" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B151" s="1" t="s">
         <v>73</v>
@@ -9278,7 +9278,7 @@
     </row>
     <row r="152" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A152" s="22" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="B152" s="1" t="s">
         <v>91</v>
@@ -9331,7 +9331,7 @@
     </row>
     <row r="153" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A153" s="22" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="B153" s="1" t="s">
         <v>91</v>
@@ -9382,7 +9382,7 @@
     </row>
     <row r="154" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A154" s="23" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="B154" s="21" t="s">
         <v>90</v>
@@ -9433,7 +9433,7 @@
     </row>
     <row r="155" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A155" s="22" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="B155" s="1" t="s">
         <v>101</v>
@@ -9486,7 +9486,7 @@
     </row>
     <row r="156" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A156" s="22" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="B156" s="1" t="s">
         <v>101</v>
@@ -9537,7 +9537,7 @@
     </row>
     <row r="157" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A157" s="22" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="B157" s="1" t="s">
         <v>88</v>
@@ -9588,7 +9588,7 @@
     </row>
     <row r="158" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A158" s="22" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="B158" s="1" t="s">
         <v>96</v>
@@ -9641,7 +9641,7 @@
     </row>
     <row r="159" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A159" s="22" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="B159" s="1" t="s">
         <v>96</v>
@@ -9692,7 +9692,7 @@
     </row>
     <row r="160" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A160" s="22" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="B160" s="1" t="s">
         <v>98</v>
@@ -9745,7 +9745,7 @@
     </row>
     <row r="161" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A161" s="22" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="B161" s="1" t="s">
         <v>98</v>
@@ -9796,7 +9796,7 @@
     </row>
     <row r="162" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A162" s="22" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="B162" s="1" t="s">
         <v>86</v>
@@ -9847,7 +9847,7 @@
     </row>
     <row r="163" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A163" s="22" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="B163" s="1" t="s">
         <v>100</v>
@@ -9900,7 +9900,7 @@
     </row>
     <row r="164" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A164" s="22" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="B164" s="1" t="s">
         <v>100</v>
@@ -9951,7 +9951,7 @@
     </row>
     <row r="165" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A165" s="22" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="B165" s="1" t="s">
         <v>89</v>
@@ -10002,7 +10002,7 @@
     </row>
     <row r="166" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A166" s="22" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="B166" s="1" t="s">
         <v>99</v>
@@ -10055,7 +10055,7 @@
     </row>
     <row r="167" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A167" s="22" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="B167" s="1" t="s">
         <v>99</v>
@@ -10106,7 +10106,7 @@
     </row>
     <row r="168" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A168" s="22" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="B168" s="1" t="s">
         <v>94</v>
@@ -10157,7 +10157,7 @@
     </row>
     <row r="169" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A169" s="22" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="B169" s="1" t="s">
         <v>94</v>
@@ -10208,7 +10208,7 @@
     </row>
     <row r="170" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A170" s="22" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="B170" s="1" t="s">
         <v>87</v>
@@ -10259,7 +10259,7 @@
     </row>
     <row r="171" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A171" s="22" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="B171" s="1" t="s">
         <v>92</v>
@@ -10312,7 +10312,7 @@
     </row>
     <row r="172" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A172" s="22" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="B172" s="1" t="s">
         <v>97</v>
@@ -10363,7 +10363,7 @@
     </row>
     <row r="173" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A173" s="22" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="B173" s="1" t="s">
         <v>97</v>
@@ -10414,7 +10414,7 @@
     </row>
     <row r="174" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A174" s="22" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="B174" s="1" t="s">
         <v>91</v>
@@ -10467,7 +10467,7 @@
     </row>
     <row r="175" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A175" s="22" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="B175" s="1" t="s">
         <v>95</v>
@@ -10520,7 +10520,7 @@
     </row>
     <row r="176" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A176" s="22" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="B176" s="1" t="s">
         <v>95</v>
@@ -10571,7 +10571,7 @@
     </row>
     <row r="177" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A177" s="22" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="B177" s="1" t="s">
         <v>93</v>
@@ -10622,7 +10622,7 @@
     </row>
     <row r="178" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A178" s="22" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B178" s="1" t="s">
         <v>72</v>
@@ -10673,7 +10673,7 @@
     </row>
     <row r="179" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A179" s="22" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B179" s="1" t="s">
         <v>72</v>
@@ -10724,7 +10724,7 @@
     </row>
     <row r="180" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A180" s="22" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="B180" s="1" t="s">
         <v>101</v>
@@ -10775,7 +10775,7 @@
     </row>
     <row r="181" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A181" s="22" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B181" s="1" t="s">
         <v>78</v>
@@ -10828,7 +10828,7 @@
     </row>
     <row r="182" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A182" s="22" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B182" s="1" t="s">
         <v>78</v>
@@ -10879,7 +10879,7 @@
     </row>
     <row r="183" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A183" s="22" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="B183" s="1" t="s">
         <v>83</v>
@@ -10932,7 +10932,7 @@
     </row>
     <row r="184" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A184" s="22" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="B184" s="1" t="s">
         <v>83</v>
@@ -10983,7 +10983,7 @@
     </row>
     <row r="185" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A185" s="22" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="B185" s="1" t="s">
         <v>96</v>
@@ -11034,7 +11034,7 @@
     </row>
     <row r="186" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A186" s="22" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="B186" s="1" t="s">
         <v>98</v>
@@ -11085,7 +11085,7 @@
     </row>
     <row r="187" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A187" s="22" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="B187" s="1" t="s">
         <v>81</v>
@@ -11138,7 +11138,7 @@
     </row>
     <row r="188" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A188" s="22" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="B188" s="1" t="s">
         <v>81</v>
@@ -11189,7 +11189,7 @@
     </row>
     <row r="189" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A189" s="22" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B189" s="1" t="s">
         <v>74</v>
@@ -11240,7 +11240,7 @@
     </row>
     <row r="190" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A190" s="22" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B190" s="1" t="s">
         <v>74</v>
@@ -11291,7 +11291,7 @@
     </row>
     <row r="191" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A191" s="22" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="B191" s="1" t="s">
         <v>100</v>
@@ -11344,7 +11344,7 @@
     </row>
     <row r="192" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A192" s="22" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B192" s="1" t="s">
         <v>76</v>
@@ -11397,7 +11397,7 @@
     </row>
     <row r="193" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A193" s="22" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B193" s="1" t="s">
         <v>76</v>
@@ -11448,7 +11448,7 @@
     </row>
     <row r="194" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A194" s="22" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="B194" s="1" t="s">
         <v>99</v>
@@ -11499,7 +11499,7 @@
     </row>
     <row r="195" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A195" s="22" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="B195" s="1" t="s">
         <v>95</v>
@@ -11550,7 +11550,7 @@
     </row>
     <row r="196" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A196" s="22" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B196" s="1" t="s">
         <v>71</v>
@@ -11603,7 +11603,7 @@
     </row>
     <row r="197" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A197" s="22" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B197" s="1" t="s">
         <v>71</v>
@@ -11654,7 +11654,7 @@
     </row>
     <row r="198" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A198" s="29" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="B198" s="30" t="s">
         <v>56</v>
@@ -11705,7 +11705,7 @@
     </row>
     <row r="199" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A199" s="22" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="B199" s="1" t="s">
         <v>94</v>
@@ -11758,7 +11758,7 @@
     </row>
     <row r="200" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A200" s="29" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="B200" s="30" t="s">
         <v>57</v>
@@ -11809,7 +11809,7 @@
     </row>
     <row r="201" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A201" s="22" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="B201" s="1" t="s">
         <v>97</v>
@@ -11862,7 +11862,7 @@
     </row>
     <row r="202" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A202" s="22" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B202" s="1" t="s">
         <v>80</v>
@@ -11915,7 +11915,7 @@
     </row>
     <row r="203" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A203" s="22" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B203" s="1" t="s">
         <v>80</v>
@@ -11966,7 +11966,7 @@
     </row>
     <row r="204" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A204" s="29" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="B204" s="30" t="s">
         <v>53</v>
@@ -12017,7 +12017,7 @@
     </row>
     <row r="205" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A205" s="31" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="B205" s="32" t="s">
         <v>54</v>
@@ -12068,7 +12068,7 @@
     </row>
     <row r="206" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A206" s="29" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="B206" s="30" t="s">
         <v>57</v>
@@ -12119,7 +12119,7 @@
     </row>
     <row r="207" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A207" s="22" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B207" s="1" t="s">
         <v>82</v>
@@ -12172,7 +12172,7 @@
     </row>
     <row r="208" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A208" s="22" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B208" s="1" t="s">
         <v>82</v>
@@ -12223,7 +12223,7 @@
     </row>
     <row r="209" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A209" s="22" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B209" s="1" t="s">
         <v>71</v>
@@ -12274,7 +12274,7 @@
     </row>
     <row r="210" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A210" s="22" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B210" s="1" t="s">
         <v>79</v>
@@ -12327,7 +12327,7 @@
     </row>
     <row r="211" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A211" s="22" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B211" s="1" t="s">
         <v>79</v>
@@ -12378,7 +12378,7 @@
     </row>
     <row r="212" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A212" s="29" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="B212" s="30" t="s">
         <v>56</v>
@@ -12429,7 +12429,7 @@
     </row>
     <row r="213" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A213" s="22" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B213" s="1" t="s">
         <v>76</v>
@@ -12480,7 +12480,7 @@
     </row>
     <row r="214" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A214" s="22" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="B214" s="1" t="s">
         <v>85</v>
@@ -12533,7 +12533,7 @@
     </row>
     <row r="215" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A215" s="22" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="B215" s="1" t="s">
         <v>85</v>
@@ -12584,7 +12584,7 @@
     </row>
     <row r="216" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A216" s="22" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B216" s="1" t="s">
         <v>72</v>
@@ -12637,10 +12637,10 @@
     </row>
     <row r="217" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A217" s="22" t="s">
-        <v>139</v>
+        <v>113</v>
       </c>
       <c r="B217" s="1" t="s">
-        <v>140</v>
+        <v>102</v>
       </c>
       <c r="C217" s="6" t="s">
         <v>2</v>
@@ -12690,10 +12690,10 @@
     </row>
     <row r="218" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A218" s="22" t="s">
-        <v>139</v>
+        <v>113</v>
       </c>
       <c r="B218" s="1" t="s">
-        <v>140</v>
+        <v>102</v>
       </c>
       <c r="C218" s="6" t="s">
         <v>1</v>
@@ -12741,7 +12741,7 @@
     </row>
     <row r="219" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A219" s="22" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="B219" s="1" t="s">
         <v>84</v>
@@ -12792,7 +12792,7 @@
     </row>
     <row r="220" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A220" s="22" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="B220" s="1" t="s">
         <v>84</v>
@@ -12843,7 +12843,7 @@
     </row>
     <row r="221" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A221" s="22" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="B221" s="1" t="s">
         <v>83</v>
@@ -12894,7 +12894,7 @@
     </row>
     <row r="222" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A222" s="22" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B222" s="1" t="s">
         <v>75</v>
@@ -12947,7 +12947,7 @@
     </row>
     <row r="223" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A223" s="22" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B223" s="1" t="s">
         <v>75</v>
@@ -12998,7 +12998,7 @@
     </row>
     <row r="224" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A224" s="22" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B224" s="1" t="s">
         <v>80</v>
@@ -13051,7 +13051,7 @@
     </row>
     <row r="225" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A225" s="22" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B225" s="1" t="s">
         <v>73</v>
@@ -13104,7 +13104,7 @@
     </row>
     <row r="226" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A226" s="22" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B226" s="1" t="s">
         <v>73</v>
@@ -13155,7 +13155,7 @@
     </row>
     <row r="227" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A227" s="22" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B227" s="1" t="s">
         <v>74</v>
@@ -13206,7 +13206,7 @@
     </row>
     <row r="228" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A228" s="22" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B228" s="1" t="s">
         <v>78</v>
@@ -13257,7 +13257,7 @@
     </row>
     <row r="229" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A229" s="22" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B229" s="1" t="s">
         <v>77</v>
@@ -13308,7 +13308,7 @@
     </row>
     <row r="230" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A230" s="22" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B230" s="1" t="s">
         <v>77</v>
@@ -13359,7 +13359,7 @@
     </row>
     <row r="231" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A231" s="22" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="B231" s="1" t="s">
         <v>81</v>
@@ -13412,7 +13412,7 @@
     </row>
     <row r="232" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A232" s="22" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="B232" s="1" t="s">
         <v>92</v>
@@ -13463,7 +13463,7 @@
     </row>
     <row r="233" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A233" s="22" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="B233" s="1" t="s">
         <v>92</v>
@@ -13514,7 +13514,7 @@
     </row>
     <row r="234" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A234" s="22" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B234" s="1" t="s">
         <v>82</v>
@@ -13565,7 +13565,7 @@
     </row>
     <row r="235" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A235" s="22" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="B235" s="1" t="s">
         <v>91</v>
@@ -13618,7 +13618,7 @@
     </row>
     <row r="236" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A236" s="22" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="B236" s="1" t="s">
         <v>91</v>
@@ -13669,7 +13669,7 @@
     </row>
     <row r="237" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A237" s="22" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="B237" s="1" t="s">
         <v>93</v>
@@ -13720,7 +13720,7 @@
     </row>
     <row r="238" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A238" s="22" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="B238" s="1" t="s">
         <v>93</v>
@@ -13771,7 +13771,7 @@
     </row>
     <row r="239" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A239" s="22" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B239" s="1" t="s">
         <v>79</v>
@@ -13824,7 +13824,7 @@
     </row>
     <row r="240" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A240" s="22" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="B240" s="1" t="s">
         <v>90</v>
@@ -13877,7 +13877,7 @@
     </row>
     <row r="241" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A241" s="22" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="B241" s="1" t="s">
         <v>90</v>
@@ -13928,7 +13928,7 @@
     </row>
     <row r="242" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A242" s="22" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="B242" s="1" t="s">
         <v>89</v>
@@ -13981,7 +13981,7 @@
     </row>
     <row r="243" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A243" s="22" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="B243" s="1" t="s">
         <v>89</v>
@@ -14032,7 +14032,7 @@
     </row>
     <row r="244" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A244" s="22" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="B244" s="1" t="s">
         <v>85</v>
@@ -14083,10 +14083,10 @@
     </row>
     <row r="245" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A245" s="22" t="s">
-        <v>139</v>
+        <v>113</v>
       </c>
       <c r="B245" s="1" t="s">
-        <v>140</v>
+        <v>102</v>
       </c>
       <c r="C245" s="6" t="s">
         <v>1</v>
@@ -14134,7 +14134,7 @@
     </row>
     <row r="246" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A246" s="22" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B246" s="1" t="s">
         <v>73</v>
@@ -14185,7 +14185,7 @@
     </row>
     <row r="247" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A247" s="22" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="B247" s="1" t="s">
         <v>87</v>
@@ -14238,7 +14238,7 @@
     </row>
     <row r="248" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A248" s="22" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="B248" s="1" t="s">
         <v>87</v>
@@ -14289,7 +14289,7 @@
     </row>
     <row r="249" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A249" s="22" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="B249" s="1" t="s">
         <v>84</v>
@@ -14340,7 +14340,7 @@
     </row>
     <row r="250" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A250" s="22" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="B250" s="1" t="s">
         <v>86</v>
@@ -14393,7 +14393,7 @@
     </row>
     <row r="251" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A251" s="22" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="B251" s="1" t="s">
         <v>86</v>
@@ -14444,7 +14444,7 @@
     </row>
     <row r="252" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A252" s="22" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B252" s="1" t="s">
         <v>75</v>
@@ -14495,7 +14495,7 @@
     </row>
     <row r="253" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A253" s="22" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B253" s="1" t="s">
         <v>77</v>
@@ -14546,7 +14546,7 @@
     </row>
     <row r="254" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A254" s="22" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="B254" s="1" t="s">
         <v>88</v>
@@ -14597,7 +14597,7 @@
     </row>
     <row r="255" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A255" s="22" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="B255" s="1" t="s">
         <v>88</v>
@@ -14648,7 +14648,7 @@
     </row>
     <row r="256" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A256" s="31" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="B256" s="32" t="s">
         <v>54</v>
@@ -14699,7 +14699,7 @@
     </row>
     <row r="257" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A257" s="22" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="B257" s="1" t="s">
         <v>88</v>
@@ -14750,7 +14750,7 @@
     </row>
     <row r="258" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A258" s="22" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="B258" s="1" t="s">
         <v>100</v>
@@ -14803,7 +14803,7 @@
     </row>
     <row r="259" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A259" s="22" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="B259" s="1" t="s">
         <v>100</v>
@@ -14854,7 +14854,7 @@
     </row>
     <row r="260" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A260" s="22" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="B260" s="1" t="s">
         <v>92</v>
@@ -14905,7 +14905,7 @@
     </row>
     <row r="261" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A261" s="22" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="B261" s="1" t="s">
         <v>101</v>
@@ -14958,7 +14958,7 @@
     </row>
     <row r="262" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A262" s="22" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="B262" s="1" t="s">
         <v>101</v>
@@ -15009,7 +15009,7 @@
     </row>
     <row r="263" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A263" s="29" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="B263" s="30" t="s">
         <v>53</v>
@@ -15060,7 +15060,7 @@
     </row>
     <row r="264" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A264" s="22" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="B264" s="1" t="s">
         <v>99</v>
@@ -15111,7 +15111,7 @@
     </row>
     <row r="265" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A265" s="22" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="B265" s="1" t="s">
         <v>99</v>
@@ -15162,7 +15162,7 @@
     </row>
     <row r="266" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A266" s="22" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="B266" s="1" t="s">
         <v>93</v>
@@ -15213,7 +15213,7 @@
     </row>
     <row r="267" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A267" s="22" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="B267" s="1" t="s">
         <v>96</v>
@@ -15266,7 +15266,7 @@
     </row>
     <row r="268" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A268" s="22" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="B268" s="1" t="s">
         <v>96</v>
@@ -15317,7 +15317,7 @@
     </row>
     <row r="269" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A269" s="22" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="B269" s="1" t="s">
         <v>90</v>
@@ -15368,7 +15368,7 @@
     </row>
     <row r="270" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A270" s="22" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="B270" s="1" t="s">
         <v>89</v>
@@ -15419,7 +15419,7 @@
     </row>
     <row r="271" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A271" s="22" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="B271" s="1" t="s">
         <v>95</v>
@@ -15472,7 +15472,7 @@
     </row>
     <row r="272" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A272" s="22" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="B272" s="1" t="s">
         <v>95</v>
@@ -15523,7 +15523,7 @@
     </row>
     <row r="273" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A273" s="22" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="B273" s="1" t="s">
         <v>97</v>
@@ -15574,7 +15574,7 @@
     </row>
     <row r="274" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A274" s="22" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="B274" s="1" t="s">
         <v>97</v>
@@ -15625,7 +15625,7 @@
     </row>
     <row r="275" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A275" s="22" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="B275" s="1" t="s">
         <v>87</v>
@@ -15676,7 +15676,7 @@
     </row>
     <row r="276" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A276" s="29" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="B276" s="30" t="s">
         <v>55</v>
@@ -15727,7 +15727,7 @@
     </row>
     <row r="277" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A277" s="22" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="B277" s="1" t="s">
         <v>94</v>
@@ -15780,7 +15780,7 @@
     </row>
     <row r="278" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A278" s="22" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="B278" s="1" t="s">
         <v>94</v>
@@ -15831,7 +15831,7 @@
     </row>
     <row r="279" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A279" s="22" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="B279" s="1" t="s">
         <v>86</v>
@@ -15882,7 +15882,7 @@
     </row>
     <row r="280" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A280" s="22" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="B280" s="1" t="s">
         <v>98</v>
@@ -15935,7 +15935,7 @@
     </row>
     <row r="281" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A281" s="22" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="B281" s="1" t="s">
         <v>98</v>
@@ -15986,7 +15986,7 @@
     </row>
     <row r="282" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A282" s="22" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="B282" s="1" t="s">
         <v>91</v>
@@ -16039,7 +16039,7 @@
     </row>
     <row r="283" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A283" s="22" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="B283" s="1" t="s">
         <v>100</v>
@@ -16090,7 +16090,7 @@
     </row>
     <row r="284" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A284" s="22" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B284" s="1" t="s">
         <v>71</v>
@@ -16143,7 +16143,7 @@
     </row>
     <row r="285" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A285" s="22" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B285" s="1" t="s">
         <v>71</v>
@@ -16194,7 +16194,7 @@
     </row>
     <row r="286" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A286" s="22" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B286" s="1" t="s">
         <v>76</v>
@@ -16247,7 +16247,7 @@
     </row>
     <row r="287" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A287" s="22" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B287" s="1" t="s">
         <v>76</v>
@@ -16298,7 +16298,7 @@
     </row>
     <row r="288" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A288" s="22" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="B288" s="1" t="s">
         <v>101</v>
@@ -16349,7 +16349,7 @@
     </row>
     <row r="289" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A289" s="22" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B289" s="1" t="s">
         <v>72</v>
@@ -16402,7 +16402,7 @@
     </row>
     <row r="290" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A290" s="22" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B290" s="1" t="s">
         <v>72</v>
@@ -16453,7 +16453,7 @@
     </row>
     <row r="291" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A291" s="22" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="B291" s="1" t="s">
         <v>83</v>
@@ -16504,7 +16504,7 @@
     </row>
     <row r="292" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A292" s="22" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="B292" s="1" t="s">
         <v>83</v>
@@ -16555,7 +16555,7 @@
     </row>
     <row r="293" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A293" s="22" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="B293" s="1" t="s">
         <v>99</v>
@@ -16606,7 +16606,7 @@
     </row>
     <row r="294" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A294" s="22" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B294" s="1" t="s">
         <v>80</v>
@@ -16659,7 +16659,7 @@
     </row>
     <row r="295" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A295" s="22" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B295" s="1" t="s">
         <v>80</v>
@@ -16710,7 +16710,7 @@
     </row>
     <row r="296" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A296" s="22" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="B296" s="1" t="s">
         <v>95</v>
@@ -16761,7 +16761,7 @@
     </row>
     <row r="297" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A297" s="22" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="B297" s="1" t="s">
         <v>96</v>
@@ -16812,7 +16812,7 @@
     </row>
     <row r="298" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A298" s="22" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B298" s="1" t="s">
         <v>74</v>
@@ -16865,7 +16865,7 @@
     </row>
     <row r="299" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A299" s="22" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B299" s="1" t="s">
         <v>74</v>
@@ -16916,7 +16916,7 @@
     </row>
     <row r="300" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A300" s="22" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="B300" s="1" t="s">
         <v>97</v>
@@ -16967,7 +16967,7 @@
     </row>
     <row r="301" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A301" s="22" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="B301" s="1" t="s">
         <v>94</v>
@@ -17020,7 +17020,7 @@
     </row>
     <row r="302" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A302" s="22" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B302" s="1" t="s">
         <v>78</v>
@@ -17073,7 +17073,7 @@
     </row>
     <row r="303" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A303" s="22" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B303" s="1" t="s">
         <v>78</v>
@@ -17124,7 +17124,7 @@
     </row>
     <row r="304" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A304" s="22" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="B304" s="1" t="s">
         <v>81</v>
@@ -17175,7 +17175,7 @@
     </row>
     <row r="305" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A305" s="22" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="B305" s="1" t="s">
         <v>81</v>
@@ -17226,7 +17226,7 @@
     </row>
     <row r="306" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A306" s="29" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="B306" s="30" t="s">
         <v>52</v>
@@ -17277,7 +17277,7 @@
     </row>
     <row r="307" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A307" s="23" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="B307" s="21" t="s">
         <v>98</v>
@@ -17328,7 +17328,7 @@
     </row>
     <row r="308" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A308" s="29" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="B308" s="30" t="s">
         <v>52</v>
@@ -17379,7 +17379,7 @@
     </row>
     <row r="309" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A309" s="29" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="B309" s="30" t="s">
         <v>53</v>
@@ -17430,7 +17430,7 @@
     </row>
     <row r="310" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A310" s="22" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="B310" s="1" t="s">
         <v>84</v>
@@ -17483,7 +17483,7 @@
     </row>
     <row r="311" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A311" s="22" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="B311" s="1" t="s">
         <v>84</v>
@@ -17534,7 +17534,7 @@
     </row>
     <row r="312" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A312" s="22" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B312" s="1" t="s">
         <v>74</v>
@@ -17585,10 +17585,10 @@
     </row>
     <row r="313" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A313" s="22" t="s">
-        <v>139</v>
+        <v>113</v>
       </c>
       <c r="B313" s="1" t="s">
-        <v>140</v>
+        <v>102</v>
       </c>
       <c r="C313" s="6" t="s">
         <v>1</v>
@@ -17638,10 +17638,10 @@
     </row>
     <row r="314" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A314" s="22" t="s">
-        <v>139</v>
+        <v>113</v>
       </c>
       <c r="B314" s="1" t="s">
-        <v>140</v>
+        <v>102</v>
       </c>
       <c r="C314" s="11" t="s">
         <v>1</v>
@@ -17689,7 +17689,7 @@
     </row>
     <row r="315" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A315" s="22" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="B315" s="1" t="s">
         <v>83</v>
@@ -17742,7 +17742,7 @@
     </row>
     <row r="316" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A316" s="22" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B316" s="1" t="s">
         <v>79</v>
@@ -17793,7 +17793,7 @@
     </row>
     <row r="317" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A317" s="22" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B317" s="1" t="s">
         <v>79</v>
@@ -17844,7 +17844,7 @@
     </row>
     <row r="318" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A318" s="22" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="B318" s="1" t="s">
         <v>81</v>
@@ -17895,7 +17895,7 @@
     </row>
     <row r="319" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A319" s="22" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B319" s="1" t="s">
         <v>82</v>
@@ -17948,7 +17948,7 @@
     </row>
     <row r="320" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A320" s="22" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B320" s="1" t="s">
         <v>82</v>
@@ -17999,7 +17999,7 @@
     </row>
     <row r="321" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A321" s="22" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B321" s="1" t="s">
         <v>71</v>
@@ -18050,7 +18050,7 @@
     </row>
     <row r="322" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A322" s="22" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B322" s="1" t="s">
         <v>73</v>
@@ -18101,7 +18101,7 @@
     </row>
     <row r="323" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A323" s="22" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B323" s="1" t="s">
         <v>73</v>
@@ -18152,7 +18152,7 @@
     </row>
     <row r="324" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A324" s="22" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="B324" s="1" t="s">
         <v>85</v>
@@ -18205,7 +18205,7 @@
     </row>
     <row r="325" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A325" s="22" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="B325" s="1" t="s">
         <v>85</v>
@@ -18256,7 +18256,7 @@
     </row>
     <row r="326" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A326" s="22" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B326" s="1" t="s">
         <v>72</v>
@@ -18307,7 +18307,7 @@
     </row>
     <row r="327" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A327" s="22" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B327" s="1" t="s">
         <v>80</v>
@@ -18358,7 +18358,7 @@
     </row>
     <row r="328" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A328" s="22" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B328" s="1" t="s">
         <v>77</v>
@@ -18411,7 +18411,7 @@
     </row>
     <row r="329" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A329" s="22" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B329" s="1" t="s">
         <v>77</v>
@@ -18462,7 +18462,7 @@
     </row>
     <row r="330" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A330" s="22" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B330" s="1" t="s">
         <v>78</v>
@@ -18515,7 +18515,7 @@
     </row>
     <row r="331" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A331" s="22" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B331" s="1" t="s">
         <v>76</v>
@@ -18568,7 +18568,7 @@
     </row>
     <row r="332" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A332" s="22" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B332" s="1" t="s">
         <v>75</v>
@@ -18621,7 +18621,7 @@
     </row>
     <row r="333" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A333" s="22" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B333" s="1" t="s">
         <v>75</v>
@@ -18672,7 +18672,7 @@
     </row>
     <row r="334" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A334" s="22" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="B334" s="1" t="s">
         <v>84</v>
@@ -18723,7 +18723,7 @@
     </row>
     <row r="335" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A335" s="22" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="B335" s="1" t="s">
         <v>93</v>
@@ -18776,7 +18776,7 @@
     </row>
     <row r="336" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A336" s="22" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="B336" s="1" t="s">
         <v>93</v>
@@ -18827,10 +18827,10 @@
     </row>
     <row r="337" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A337" s="22" t="s">
-        <v>139</v>
+        <v>113</v>
       </c>
       <c r="B337" s="1" t="s">
-        <v>140</v>
+        <v>102</v>
       </c>
       <c r="C337" s="6" t="s">
         <v>1</v>
@@ -18878,7 +18878,7 @@
     </row>
     <row r="338" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A338" s="22" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="B338" s="1" t="s">
         <v>89</v>
@@ -18931,7 +18931,7 @@
     </row>
     <row r="339" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A339" s="22" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="B339" s="1" t="s">
         <v>89</v>
@@ -18982,7 +18982,7 @@
     </row>
     <row r="340" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A340" s="22" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B340" s="1" t="s">
         <v>82</v>
@@ -19033,7 +19033,7 @@
     </row>
     <row r="341" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A341" s="22" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="B341" s="1" t="s">
         <v>91</v>
@@ -19084,7 +19084,7 @@
     </row>
     <row r="342" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A342" s="22" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="B342" s="1" t="s">
         <v>91</v>
@@ -19135,7 +19135,7 @@
     </row>
     <row r="343" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A343" s="22" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="B343" s="1" t="s">
         <v>87</v>
@@ -19188,7 +19188,7 @@
     </row>
     <row r="344" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A344" s="22" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="B344" s="1" t="s">
         <v>87</v>
@@ -19239,7 +19239,7 @@
     </row>
     <row r="345" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A345" s="22" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B345" s="1" t="s">
         <v>79</v>
@@ -19290,7 +19290,7 @@
     </row>
     <row r="346" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A346" s="22" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="B346" s="1" t="s">
         <v>92</v>
@@ -19343,7 +19343,7 @@
     </row>
     <row r="347" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A347" s="22" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="B347" s="1" t="s">
         <v>92</v>
@@ -19394,7 +19394,7 @@
     </row>
     <row r="348" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A348" s="22" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B348" s="1" t="s">
         <v>77</v>
@@ -19445,7 +19445,7 @@
     </row>
     <row r="349" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A349" s="22" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B349" s="1" t="s">
         <v>73</v>
@@ -19498,7 +19498,7 @@
     </row>
     <row r="350" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A350" s="22" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="B350" s="1" t="s">
         <v>88</v>
@@ -19551,7 +19551,7 @@
     </row>
     <row r="351" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A351" s="22" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="B351" s="1" t="s">
         <v>88</v>
@@ -19602,7 +19602,7 @@
     </row>
     <row r="352" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A352" s="22" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="B352" s="1" t="s">
         <v>85</v>
@@ -19653,7 +19653,7 @@
     </row>
     <row r="353" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A353" s="22" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="B353" s="1" t="s">
         <v>90</v>
@@ -19706,7 +19706,7 @@
     </row>
     <row r="354" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A354" s="22" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="B354" s="1" t="s">
         <v>90</v>
@@ -19757,7 +19757,7 @@
     </row>
     <row r="355" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A355" s="29" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="B355" s="30" t="s">
         <v>54</v>
@@ -19808,7 +19808,7 @@
     </row>
     <row r="356" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A356" s="22" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B356" s="1" t="s">
         <v>75</v>
@@ -19859,7 +19859,7 @@
     </row>
     <row r="357" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A357" s="22" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="B357" s="1" t="s">
         <v>86</v>
@@ -19912,7 +19912,7 @@
     </row>
     <row r="358" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A358" s="23" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="B358" s="21" t="s">
         <v>86</v>
@@ -19963,7 +19963,7 @@
     </row>
     <row r="359" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A359" s="22" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="B359" s="1" t="s">
         <v>95</v>
@@ -20014,7 +20014,7 @@
     </row>
     <row r="360" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A360" s="22" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="B360" s="1" t="s">
         <v>95</v>
@@ -20065,7 +20065,7 @@
     </row>
     <row r="361" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A361" s="29" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="B361" s="30" t="s">
         <v>55</v>
@@ -20116,7 +20116,7 @@
     </row>
     <row r="362" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A362" s="22" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="B362" s="1" t="s">
         <v>98</v>
@@ -20169,7 +20169,7 @@
     </row>
     <row r="363" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A363" s="22" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="B363" s="1" t="s">
         <v>98</v>
@@ -20220,7 +20220,7 @@
     </row>
     <row r="364" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A364" s="22" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="B364" s="1" t="s">
         <v>93</v>
@@ -20273,7 +20273,7 @@
     </row>
     <row r="365" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A365" s="22" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="B365" s="1" t="s">
         <v>97</v>
@@ -20326,7 +20326,7 @@
     </row>
     <row r="366" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A366" s="22" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="B366" s="1" t="s">
         <v>97</v>
@@ -20377,7 +20377,7 @@
     </row>
     <row r="367" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A367" s="22" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="B367" s="1" t="s">
         <v>89</v>
@@ -20428,7 +20428,7 @@
     </row>
     <row r="368" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A368" s="22" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="B368" s="1" t="s">
         <v>87</v>
@@ -20479,7 +20479,7 @@
     </row>
     <row r="369" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A369" s="22" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="B369" s="1" t="s">
         <v>101</v>
@@ -20532,7 +20532,7 @@
     </row>
     <row r="370" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A370" s="22" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="B370" s="1" t="s">
         <v>101</v>
@@ -20583,7 +20583,7 @@
     </row>
     <row r="371" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A371" s="22" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="B371" s="1" t="s">
         <v>92</v>
@@ -20634,7 +20634,7 @@
     </row>
     <row r="372" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A372" s="22" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="B372" s="1" t="s">
         <v>88</v>
@@ -20687,7 +20687,7 @@
     </row>
     <row r="373" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A373" s="22" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="B373" s="1" t="s">
         <v>94</v>
@@ -20740,7 +20740,7 @@
     </row>
     <row r="374" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A374" s="22" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="B374" s="1" t="s">
         <v>94</v>
@@ -20791,7 +20791,7 @@
     </row>
     <row r="375" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A375" s="29" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="B375" s="30" t="s">
         <v>56</v>
@@ -20842,7 +20842,7 @@
     </row>
     <row r="376" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A376" s="22" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="B376" s="1" t="s">
         <v>100</v>
@@ -20893,7 +20893,7 @@
     </row>
     <row r="377" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A377" s="22" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="B377" s="1" t="s">
         <v>100</v>
@@ -20944,7 +20944,7 @@
     </row>
     <row r="378" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A378" s="22" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="B378" s="1" t="s">
         <v>91</v>
@@ -20995,7 +20995,7 @@
     </row>
     <row r="379" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A379" s="22" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="B379" s="1" t="s">
         <v>96</v>
@@ -21048,7 +21048,7 @@
     </row>
     <row r="380" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A380" s="22" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="B380" s="1" t="s">
         <v>96</v>
@@ -21099,7 +21099,7 @@
     </row>
     <row r="381" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A381" s="22" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="B381" s="1" t="s">
         <v>90</v>
@@ -21150,7 +21150,7 @@
     </row>
     <row r="382" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A382" s="22" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="B382" s="1" t="s">
         <v>86</v>
@@ -21203,7 +21203,7 @@
     </row>
     <row r="383" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A383" s="22" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="B383" s="1" t="s">
         <v>99</v>
@@ -21256,7 +21256,7 @@
     </row>
     <row r="384" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A384" s="22" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="B384" s="1" t="s">
         <v>99</v>
@@ -21307,7 +21307,7 @@
     </row>
     <row r="385" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A385" s="22" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="B385" s="1" t="s">
         <v>95</v>
@@ -21358,7 +21358,7 @@
     </row>
     <row r="386" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A386" s="22" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B386" s="1" t="s">
         <v>74</v>
@@ -21411,7 +21411,7 @@
     </row>
     <row r="387" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A387" s="22" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B387" s="1" t="s">
         <v>74</v>
@@ -21462,7 +21462,7 @@
     </row>
     <row r="388" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A388" s="22" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="B388" s="1" t="s">
         <v>83</v>
@@ -21513,7 +21513,7 @@
     </row>
     <row r="389" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A389" s="22" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="B389" s="1" t="s">
         <v>83</v>
@@ -21564,7 +21564,7 @@
     </row>
     <row r="390" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A390" s="22" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="B390" s="1" t="s">
         <v>97</v>
@@ -21617,7 +21617,7 @@
     </row>
     <row r="391" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A391" s="22" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="B391" s="1" t="s">
         <v>98</v>
@@ -21668,7 +21668,7 @@
     </row>
     <row r="392" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A392" s="22" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B392" s="1" t="s">
         <v>71</v>
@@ -21721,7 +21721,7 @@
     </row>
     <row r="393" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A393" s="22" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B393" s="1" t="s">
         <v>71</v>
@@ -21772,7 +21772,7 @@
     </row>
     <row r="394" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A394" s="22" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B394" s="1" t="s">
         <v>72</v>
@@ -21825,7 +21825,7 @@
     </row>
     <row r="395" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A395" s="22" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B395" s="1" t="s">
         <v>72</v>
@@ -21876,7 +21876,7 @@
     </row>
     <row r="396" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A396" s="22" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="B396" s="1" t="s">
         <v>101</v>
@@ -21927,7 +21927,7 @@
     </row>
     <row r="397" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A397" s="22" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="B397" s="1" t="s">
         <v>94</v>
@@ -21978,7 +21978,7 @@
     </row>
     <row r="398" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A398" s="22" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="B398" s="1" t="s">
         <v>81</v>
@@ -22031,7 +22031,7 @@
     </row>
     <row r="399" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A399" s="22" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="B399" s="1" t="s">
         <v>81</v>
@@ -22082,7 +22082,7 @@
     </row>
     <row r="400" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A400" s="22" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B400" s="1" t="s">
         <v>78</v>
@@ -22133,7 +22133,7 @@
     </row>
     <row r="401" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A401" s="22" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B401" s="1" t="s">
         <v>78</v>
@@ -22184,7 +22184,7 @@
     </row>
     <row r="402" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A402" s="29" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="B402" s="30" t="s">
         <v>57</v>
@@ -22235,7 +22235,7 @@
     </row>
     <row r="403" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A403" s="22" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="B403" s="1" t="s">
         <v>96</v>
@@ -22286,7 +22286,7 @@
     </row>
     <row r="404" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A404" s="22" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B404" s="1" t="s">
         <v>80</v>
@@ -22337,7 +22337,7 @@
     </row>
     <row r="405" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A405" s="22" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B405" s="1" t="s">
         <v>80</v>
@@ -22388,7 +22388,7 @@
     </row>
     <row r="406" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A406" s="22" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B406" s="1" t="s">
         <v>76</v>
@@ -22439,7 +22439,7 @@
     </row>
     <row r="407" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A407" s="22" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B407" s="1" t="s">
         <v>76</v>
@@ -22490,7 +22490,7 @@
     </row>
     <row r="408" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A408" s="22" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="B408" s="1" t="s">
         <v>99</v>
@@ -22541,7 +22541,7 @@
     </row>
     <row r="409" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A409" s="22" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="B409" s="1" t="s">
         <v>100</v>

</xml_diff>